<commit_message>
feat: refactored eurostat import
</commit_message>
<xml_diff>
--- a/import/raw_data/eurostat/mapping__nrg_bal__parameter.xlsx
+++ b/import/raw_data/eurostat/mapping__nrg_bal__parameter.xlsx
@@ -1,32 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_env\workspace\micat\back_end\import\public\eurostat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenz/Projekte/micat/import/raw_data/eurostat/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91674020-DF25-2C4F-8159-E97BD5BEDFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="31260" yWindow="-21160" windowWidth="27760" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1158,7 +1147,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1217,7 +1206,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1528,21 +1517,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75:C139"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="19.7109375" customWidth="1"/>
+    <col min="2" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="92" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>373</v>
       </c>
@@ -1559,7 +1548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1576,7 +1565,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1593,7 +1582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1610,7 +1599,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1627,7 +1616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1644,7 +1633,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1661,7 +1650,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1678,7 +1667,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1695,7 +1684,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1712,7 +1701,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1729,7 +1718,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1746,7 +1735,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1763,7 +1752,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1780,7 +1769,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1797,7 +1786,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1814,7 +1803,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1831,7 +1820,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1848,7 +1837,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1865,7 +1854,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1882,7 +1871,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1899,7 +1888,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1916,7 +1905,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1933,7 +1922,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1950,7 +1939,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1967,7 +1956,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1984,7 +1973,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2001,7 +1990,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2018,7 +2007,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2035,7 +2024,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2052,7 +2041,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2069,7 +2058,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2086,7 +2075,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2103,7 +2092,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2120,7 +2109,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2137,7 +2126,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2154,7 +2143,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2171,7 +2160,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2185,7 +2174,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2199,7 +2188,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2213,7 +2202,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2227,7 +2216,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2241,7 +2230,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2255,7 +2244,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2269,7 +2258,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2283,7 +2272,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2297,7 +2286,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2311,7 +2300,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2325,7 +2314,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2339,7 +2328,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2356,7 +2345,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2373,7 +2362,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2390,7 +2379,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2407,7 +2396,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2424,7 +2413,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2441,7 +2430,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2458,7 +2447,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2475,7 +2464,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2492,7 +2481,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2509,7 +2498,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2526,7 +2515,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2543,7 +2532,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2560,7 +2549,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2577,7 +2566,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2594,7 +2583,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2611,7 +2600,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2628,7 +2617,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2645,7 +2634,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2662,7 +2651,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2679,7 +2668,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2696,7 +2685,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2713,7 +2702,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2727,7 +2716,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2744,7 +2733,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2761,7 +2750,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2778,7 +2767,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2795,7 +2784,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2812,7 +2801,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2829,7 +2818,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2846,7 +2835,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2863,7 +2852,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2880,7 +2869,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2897,7 +2886,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2914,7 +2903,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2931,7 +2920,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2945,7 +2934,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2959,7 +2948,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2973,7 +2962,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2987,7 +2976,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3001,7 +2990,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3015,7 +3004,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3029,7 +3018,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3046,7 +3035,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3060,7 +3049,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3074,7 +3063,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3088,7 +3077,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3105,7 +3094,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3122,7 +3111,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3136,7 +3125,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3153,7 +3142,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3170,7 +3159,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3187,7 +3176,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3204,7 +3193,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3218,7 +3207,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3235,7 +3224,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3249,7 +3238,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3266,7 +3255,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3283,7 +3272,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3300,7 +3289,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3317,7 +3306,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3334,7 +3323,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3351,7 +3340,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3368,7 +3357,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3382,7 +3371,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3396,7 +3385,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3413,7 +3402,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3430,7 +3419,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3447,7 +3436,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3461,7 +3450,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3475,7 +3464,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3489,7 +3478,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3503,7 +3492,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3517,7 +3506,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -3531,7 +3520,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -3545,7 +3534,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -3559,7 +3548,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -3573,7 +3562,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3590,7 +3579,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3604,7 +3593,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3621,7 +3610,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3635,7 +3624,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3649,7 +3638,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -3666,7 +3655,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -3680,7 +3669,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -3694,7 +3683,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -3711,7 +3700,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -3728,7 +3717,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -3745,7 +3734,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -3762,7 +3751,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -3785,15 +3774,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010081027A5C4AB68A40A5017F28CDCC410C" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6a99bad85733394ec9884d367e30f22e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca47701c-f272-4f81-9665-1c7dbebc0776" xmlns:ns3="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7c78837beb47b266e55ad3edbd611a71" ns2:_="" ns3:_="">
     <xsd:import namespace="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
@@ -4040,7 +4020,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
@@ -4052,15 +4032,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A20985FE-D712-453E-8550-5ADA14768C4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A8625DA-B0C2-4D32-8FF9-32BFFC446355}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4079,7 +4060,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4BF1D79-FFAB-4BA6-BDE1-966B5659A2B6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4088,4 +4069,12 @@
     <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A20985FE-D712-453E-8550-5ADA14768C4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>